<commit_message>
tested all models and raise notimplemented for ones that don't work
</commit_message>
<xml_diff>
--- a/thunderfit/compairosn_algorithms.xlsx
+++ b/thunderfit/compairosn_algorithms.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>run time (one run on example data)</t>
   </si>
@@ -75,16 +75,99 @@
   </si>
   <si>
     <t>:0.001,</t>
+  </si>
+  <si>
+    <t>tested models</t>
+  </si>
+  <si>
+    <t>GaussianModel</t>
+  </si>
+  <si>
+    <t>LorentzianModel</t>
+  </si>
+  <si>
+    <t>SplitLorentzianModel</t>
+  </si>
+  <si>
+    <t>VoigtModel</t>
+  </si>
+  <si>
+    <t>PseudoVoigtModel</t>
+  </si>
+  <si>
+    <t>MoffatModel</t>
+  </si>
+  <si>
+    <t>Pearson7Model</t>
+  </si>
+  <si>
+    <t>StudentsTModel</t>
+  </si>
+  <si>
+    <t>BreitWignerModel</t>
+  </si>
+  <si>
+    <t>LognormalModel</t>
+  </si>
+  <si>
+    <t>DampedOcsillatorModel</t>
+  </si>
+  <si>
+    <t>DampedHarmonicOcsillatorModel</t>
+  </si>
+  <si>
+    <t>ExponentialGaussianModel</t>
+  </si>
+  <si>
+    <t>SkewedGaussianModel</t>
+  </si>
+  <si>
+    <t>SkewedVoigtModel</t>
+  </si>
+  <si>
+    <t>DonaichModel</t>
+  </si>
+  <si>
+    <t>ConstantModel</t>
+  </si>
+  <si>
+    <t>LinearModel</t>
+  </si>
+  <si>
+    <t>QuadraticModel</t>
+  </si>
+  <si>
+    <t>PolynomialModel</t>
+  </si>
+  <si>
+    <t>StepModel</t>
+  </si>
+  <si>
+    <t>RectangleModel</t>
+  </si>
+  <si>
+    <t>ExponentialModel</t>
+  </si>
+  <si>
+    <t>PowerLawModel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,13 +190,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,9 +494,10 @@
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -415,8 +507,11 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -426,8 +521,9 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -437,8 +533,11 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -448,8 +547,11 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -459,8 +561,11 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -470,8 +575,11 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -481,8 +589,11 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -492,8 +603,11 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -503,8 +617,11 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -514,8 +631,11 @@
       <c r="C10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -525,8 +645,11 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -536,8 +659,11 @@
       <c r="C12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -547,8 +673,11 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H13" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -558,8 +687,11 @@
       <c r="C14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -569,8 +701,11 @@
       <c r="C15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -580,8 +715,97 @@
       <c r="C16" t="s">
         <v>4</v>
       </c>
+      <c r="H16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" location="gaussianmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - gaussianmodel"/>
+    <hyperlink ref="H4" r:id="rId2" location="lorentzianmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - lorentzianmodel"/>
+    <hyperlink ref="H5" r:id="rId3" location="splitlorentzianmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - splitlorentzianmodel"/>
+    <hyperlink ref="H6" r:id="rId4" location="voigtmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - voigtmodel"/>
+    <hyperlink ref="H7" r:id="rId5" location="pseudovoigtmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - pseudovoigtmodel"/>
+    <hyperlink ref="H8" r:id="rId6" location="moffatmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - moffatmodel"/>
+    <hyperlink ref="H9" r:id="rId7" location="pearson7model" display="https://lmfit.github.io/lmfit-py/builtin_models.html - pearson7model"/>
+    <hyperlink ref="H10" r:id="rId8" location="studentstmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - studentstmodel"/>
+    <hyperlink ref="H11" r:id="rId9" location="breitwignermodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - breitwignermodel"/>
+    <hyperlink ref="H12" r:id="rId10" location="lognormalmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - lognormalmodel"/>
+    <hyperlink ref="H13" r:id="rId11" location="dampedocsillatormodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - dampedocsillatormodel"/>
+    <hyperlink ref="H14" r:id="rId12" location="dampedharmonicocsillatormodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - dampedharmonicocsillatormodel"/>
+    <hyperlink ref="H15" r:id="rId13" location="exponentialgaussianmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - exponentialgaussianmodel"/>
+    <hyperlink ref="H16" r:id="rId14" location="skewedgaussianmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - skewedgaussianmodel"/>
+    <hyperlink ref="H17" r:id="rId15" location="skewedvoigtmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - skewedvoigtmodel"/>
+    <hyperlink ref="H18" r:id="rId16" location="donaichmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - donaichmodel"/>
+    <hyperlink ref="H20" r:id="rId17" location="constantmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - constantmodel"/>
+    <hyperlink ref="H21" r:id="rId18" location="linearmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - linearmodel"/>
+    <hyperlink ref="H22" r:id="rId19" location="quadraticmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - quadraticmodel"/>
+    <hyperlink ref="H23" r:id="rId20" location="polynomialmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - polynomialmodel"/>
+    <hyperlink ref="H25" r:id="rId21" location="stepmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - stepmodel"/>
+    <hyperlink ref="H26" r:id="rId22" location="rectanglemodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - rectanglemodel"/>
+    <hyperlink ref="H28" r:id="rId23" location="exponentialmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - exponentialmodel"/>
+    <hyperlink ref="H29" r:id="rId24" location="powerlawmodel" display="https://lmfit.github.io/lmfit-py/builtin_models.html - powerlawmodel"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>